<commit_message>
attempt 1 to fix integration tests
</commit_message>
<xml_diff>
--- a/Documentation/Software Engineering Methods - Individual Assmement.xlsx
+++ b/Documentation/Software Engineering Methods - Individual Assmement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewsc\Desktop\sem38\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79A66B7-421B-43B4-B297-D8334BD58745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F595B117-E313-447A-A318-79B1F81E7A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C48DF21F-4747-42A5-97BD-684A76F6AE82}"/>
+    <workbookView xWindow="7870" yWindow="390" windowWidth="10930" windowHeight="9300" xr2:uid="{C48DF21F-4747-42A5-97BD-684A76F6AE82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Matriculation Number </t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Code Review 2</t>
+  </si>
+  <si>
+    <t>40724261 (Gastao Bettencourt)</t>
   </si>
 </sst>
 </file>
@@ -434,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A18B041-92FB-4AEE-A4DD-97E7115EB1EF}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="12.7265625" customWidth="1"/>
@@ -476,6 +479,9 @@
       <c r="C2">
         <v>33.299999999999997</v>
       </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -487,6 +493,9 @@
       <c r="C3">
         <v>33.299999999999997</v>
       </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -498,15 +507,36 @@
       <c r="C4">
         <v>33.299999999999997</v>
       </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>100</v>
       </c>
-      <c r="C5">
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <f>SUM(D2:D5)</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed the contributions file
</commit_message>
<xml_diff>
--- a/Documentation/Software Engineering Methods - Individual Assmement.xlsx
+++ b/Documentation/Software Engineering Methods - Individual Assmement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewsc\Desktop\sem38\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F595B117-E313-447A-A318-79B1F81E7A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B78BE7-4A6C-45E1-9593-4D0725E636A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7870" yWindow="390" windowWidth="10930" windowHeight="9300" xr2:uid="{C48DF21F-4747-42A5-97BD-684A76F6AE82}"/>
+    <workbookView xWindow="5830" yWindow="20" windowWidth="10930" windowHeight="9300" xr2:uid="{C48DF21F-4747-42A5-97BD-684A76F6AE82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,6 +482,9 @@
       <c r="D2">
         <v>30</v>
       </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -496,6 +499,9 @@
       <c r="D3">
         <v>30</v>
       </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -510,6 +516,9 @@
       <c r="D4">
         <v>30</v>
       </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -524,6 +533,9 @@
       <c r="D5">
         <v>10</v>
       </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -537,6 +549,9 @@
       </c>
       <c r="D6">
         <f>SUM(D2:D5)</f>
+        <v>100</v>
+      </c>
+      <c r="E6">
         <v>100</v>
       </c>
     </row>

</xml_diff>